<commit_message>
Figure 1 Schematic Design
Schematic design task (3), BOM file and output to pdf.
</commit_message>
<xml_diff>
--- a/Project Outputs for Worldskills Pre-Comp Task/Figure1.xlsx
+++ b/Project Outputs for Worldskills Pre-Comp Task/Figure1.xlsx
@@ -146,7 +146,7 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>330nF</t>
+    <t>1uF</t>
   </si>
   <si>
     <t>10nF</t>
@@ -209,7 +209,7 @@
     <t>9451382</t>
   </si>
   <si>
-    <t>1902922</t>
+    <t>9451358</t>
   </si>
   <si>
     <t>1216435</t>
@@ -266,7 +266,7 @@
     <t>MCGPR50V106M5X11</t>
   </si>
   <si>
-    <t>MCRH50V334M5X11</t>
+    <t>MCGPR50V105M5X11</t>
   </si>
   <si>
     <t>MCRR25103X7RK0050</t>
@@ -305,13 +305,13 @@
     <t>F:\Kerris Worldskills\CompetitionTask\Figure1.BomDoc</t>
   </si>
   <si>
-    <t>12:14:24</t>
-  </si>
-  <si>
-    <t>18/05/2018</t>
-  </si>
-  <si>
-    <t>18/05/2018 12:14:24</t>
+    <t>10:14:35</t>
+  </si>
+  <si>
+    <t>22/05/2018</t>
+  </si>
+  <si>
+    <t>22/05/2018 10:14:35</t>
   </si>
   <si>
     <t>Bill of Materials</t>
@@ -881,6 +881,18 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -920,18 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1365,7 +1365,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="34"/>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="53" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="35"/>
@@ -1416,11 +1416,11 @@
       <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="52" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="13"/>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="54" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="12"/>
@@ -1434,11 +1434,11 @@
       <c r="C4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="52" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="55" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="16"/>
@@ -1452,11 +1452,11 @@
       <c r="C5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="52" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="56" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="18"/>
@@ -1485,11 +1485,11 @@
       <c r="D7" s="22"/>
       <c r="E7" s="30">
         <f ca="1">TODAY()</f>
-        <v>43238</v>
+        <v>43242</v>
       </c>
       <c r="F7" s="31">
         <f ca="1">NOW()</f>
-        <v>43238.510076157407</v>
+        <v>43242.426823611109</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -1513,56 +1513,56 @@
       <c r="B9" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="55" t="s">
+      <c r="F9" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="55" t="s">
+      <c r="H9" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="58" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26"/>
       <c r="B10" s="47">
-        <f t="shared" ref="B10:B20" si="0">ROW(B10) - ROW($B$9)</f>
+        <f>ROW(B10) - ROW($B$9)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="61" t="s">
         <v>82</v>
       </c>
       <c r="J10" s="45">
@@ -1572,28 +1572,28 @@
     <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26"/>
       <c r="B11" s="48">
-        <f t="shared" si="0"/>
+        <f>ROW(B11) - ROW($B$9)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="62" t="s">
         <v>83</v>
       </c>
       <c r="J11" s="46">
@@ -1603,28 +1603,28 @@
     <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26"/>
       <c r="B12" s="47">
-        <f t="shared" si="0"/>
+        <f>ROW(B12) - ROW($B$9)</f>
         <v>3</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="58" t="s">
+      <c r="H12" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="61" t="s">
         <v>84</v>
       </c>
       <c r="J12" s="45">
@@ -1634,28 +1634,28 @@
     <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26"/>
       <c r="B13" s="48">
-        <f t="shared" si="0"/>
+        <f>ROW(B13) - ROW($B$9)</f>
         <v>4</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="62" t="s">
         <v>45</v>
       </c>
       <c r="J13" s="46">
@@ -1665,28 +1665,28 @@
     <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="26"/>
       <c r="B14" s="47">
-        <f t="shared" si="0"/>
+        <f>ROW(B14) - ROW($B$9)</f>
         <v>5</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="56" t="s">
+      <c r="F14" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="58" t="s">
+      <c r="H14" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="58" t="s">
+      <c r="I14" s="61" t="s">
         <v>85</v>
       </c>
       <c r="J14" s="45">
@@ -1696,28 +1696,28 @@
     <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="26"/>
       <c r="B15" s="48">
-        <f t="shared" si="0"/>
+        <f>ROW(B15) - ROW($B$9)</f>
         <v>6</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="59" t="s">
+      <c r="G15" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="62" t="s">
         <v>86</v>
       </c>
       <c r="J15" s="46">
@@ -1727,28 +1727,28 @@
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="26"/>
       <c r="B16" s="47">
-        <f t="shared" si="0"/>
+        <f>ROW(B16) - ROW($B$9)</f>
         <v>7</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="58" t="s">
+      <c r="G16" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="58" t="s">
+      <c r="H16" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="58" t="s">
+      <c r="I16" s="61" t="s">
         <v>87</v>
       </c>
       <c r="J16" s="45">
@@ -1758,28 +1758,28 @@
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="26"/>
       <c r="B17" s="48">
-        <f t="shared" si="0"/>
+        <f>ROW(B17) - ROW($B$9)</f>
         <v>8</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="F17" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I17" s="62" t="s">
         <v>88</v>
       </c>
       <c r="J17" s="46">
@@ -1789,28 +1789,28 @@
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="26"/>
       <c r="B18" s="47">
-        <f t="shared" si="0"/>
+        <f>ROW(B18) - ROW($B$9)</f>
         <v>9</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="58" t="s">
+      <c r="G18" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="H18" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="58" t="s">
+      <c r="I18" s="61" t="s">
         <v>89</v>
       </c>
       <c r="J18" s="45">
@@ -1820,28 +1820,28 @@
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="26"/>
       <c r="B19" s="48">
-        <f t="shared" si="0"/>
+        <f>ROW(B19) - ROW($B$9)</f>
         <v>10</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="D19" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="59" t="s">
+      <c r="G19" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="59" t="s">
+      <c r="H19" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I19" s="62" t="s">
         <v>90</v>
       </c>
       <c r="J19" s="46">
@@ -1851,28 +1851,28 @@
     <row r="20" spans="1:10" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="47">
-        <f t="shared" si="0"/>
+        <f>ROW(B20) - ROW($B$9)</f>
         <v>11</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="58" t="s">
+      <c r="H20" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="I20" s="58" t="s">
+      <c r="I20" s="61" t="s">
         <v>91</v>
       </c>
       <c r="J20" s="45">
@@ -1881,17 +1881,17 @@
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="54" t="s">
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="57" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G10" r:id="rId1" tooltip="Supplier" display="'9451382"/>
-    <hyperlink ref="G11" r:id="rId2" tooltip="Supplier" display="'1902922"/>
+    <hyperlink ref="G11" r:id="rId2" tooltip="Supplier" display="'9451358"/>
     <hyperlink ref="G12" r:id="rId3" tooltip="Supplier" display="'1216435"/>
     <hyperlink ref="G13" r:id="rId4" tooltip="Supplier" display="'2323100"/>
     <hyperlink ref="G14" r:id="rId5" tooltip="Supplier" display="'2314249"/>
@@ -1989,7 +1989,7 @@
     <hyperlink ref="H19" r:id="rId21" tooltip="Component" display="'TI National Semiconductor"/>
     <hyperlink ref="H20" r:id="rId22" tooltip="Component" display="'Texas Instruments"/>
     <hyperlink ref="I10" r:id="rId23" tooltip="Manufacturer" display="'MCGPR50V106M5X11"/>
-    <hyperlink ref="I11" r:id="rId24" tooltip="Manufacturer" display="'MCRH50V334M5X11"/>
+    <hyperlink ref="I11" r:id="rId24" tooltip="Manufacturer" display="'MCGPR50V105M5X11"/>
     <hyperlink ref="I12" r:id="rId25" tooltip="Manufacturer" display="'MCRR25103X7RK0050"/>
     <hyperlink ref="I13" r:id="rId26" tooltip="Manufacturer" display="'1N4001"/>
     <hyperlink ref="I14" r:id="rId27" tooltip="Manufacturer" display="'SC56-11SURKWA"/>
@@ -2028,7 +2028,7 @@
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="63" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2036,7 +2036,7 @@
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="65" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2052,7 +2052,7 @@
       <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="64" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2060,7 +2060,7 @@
       <c r="A5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="65" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
       <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="64" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2076,7 +2076,7 @@
       <c r="A7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="65" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
       <c r="A9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="65" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2100,7 +2100,7 @@
       <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="64" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2108,7 +2108,7 @@
       <c r="A11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="65" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       <c r="A12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="64" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2124,7 +2124,7 @@
       <c r="A13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="65" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2132,7 +2132,7 @@
       <c r="A14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="64" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>